<commit_message>
admin change password working
</commit_message>
<xml_diff>
--- a/misc_files/requirements_project_org_trg_breakup.xlsx
+++ b/misc_files/requirements_project_org_trg_breakup.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation Breakup" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>No</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t xml:space="preserve">Admin can generate a report of all users in the system </t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -222,6 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -533,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -544,10 +548,12 @@
     <col min="1" max="1" width="3.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="4" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="12.1640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" ht="25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,8 +563,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="E1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -568,19 +577,20 @@
       <c r="C2" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -591,7 +601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="28">
+    <row r="5" spans="1:5" s="4" customFormat="1" ht="28">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -602,7 +612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -613,7 +623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1">
+    <row r="7" spans="1:5" s="4" customFormat="1">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -621,7 +631,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28">
+    <row r="8" spans="1:5" ht="28">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -632,7 +642,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -643,7 +653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -654,7 +664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="42">
+    <row r="11" spans="1:5" ht="42">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -665,7 +675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="42">
+    <row r="12" spans="1:5" ht="42">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -676,7 +686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="42">
+    <row r="13" spans="1:5" ht="42">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -687,7 +697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28">
+    <row r="14" spans="1:5" ht="28">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -698,7 +708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28">
+    <row r="15" spans="1:5" ht="28">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -709,7 +719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28">
+    <row r="16" spans="1:5" ht="28">
       <c r="A16" s="2">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
admin org temp now persisting to db
</commit_message>
<xml_diff>
--- a/misc_files/requirements_project_org_trg_breakup.xlsx
+++ b/misc_files/requirements_project_org_trg_breakup.xlsx
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>